<commit_message>
Im fucked up Now need to rewrite everything from tommorow again or else this project is dommed
</commit_message>
<xml_diff>
--- a/examples/Risk Metrics Data.xlsx
+++ b/examples/Risk Metrics Data.xlsx
@@ -8,28 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\OneDrive\Desktop\Big Projects\FinDeck(Excel to PPT Project)\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2024CC4-CED9-4577-BA13-769B9BF43C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F33FCF-314A-46E9-BDA1-A4EBBF84A889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="4410" windowWidth="28800" windowHeight="15345" xr2:uid="{705697D5-B334-45FA-A537-E67C22AEDB59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -437,25 +423,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD26F282-7D23-4FC3-92DF-E9262E80893B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -463,7 +450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -471,7 +458,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -479,7 +466,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -487,7 +474,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>